<commit_message>
adding failed screenshot code
</commit_message>
<xml_diff>
--- a/src/main/java/Utility/ExcelData.xlsx
+++ b/src/main/java/Utility/ExcelData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d535852d4872eab2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pujap\eclipse-workspace\MavenTestify\src\main\java\Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{4620EA11-1E9F-4985-A14C-58CE604443FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13D7FDDC-184D-4297-AFF3-CCC81E3AA789}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BB1811-7E39-4A97-BE22-D76E9CAA915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC774419-47F1-47DD-8F65-561F8B4297CC}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>Test</t>
   </si>
   <si>
-    <t>testquel19@gmail.com</t>
+    <t>pooja168@givmail.com</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>